<commit_message>
Added some more columns for different areas.
</commit_message>
<xml_diff>
--- a/docs/Examples/Fitting_Water_Silicate_Melts/Example4a_H2OQuant_Glass/H2O_Silicate_areas.xlsx
+++ b/docs/Examples/Fitting_Water_Silicate_Melts/Example4a_H2OQuant_Glass/H2O_Silicate_areas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -22,73 +22,85 @@
     <t>MI filename</t>
   </si>
   <si>
+    <t>Water_to_HW_ratio_Trapezoid</t>
+  </si>
+  <si>
+    <t>Water_to_HW_ratio_Simpson</t>
+  </si>
+  <si>
+    <t>Water_to_Total_Silicate_ratio_Trapezoid</t>
+  </si>
+  <si>
+    <t>Water_to_Total_Silicate_ratio_Simpson</t>
+  </si>
+  <si>
+    <t>Water_Trapezoid_Area</t>
+  </si>
+  <si>
+    <t>Water_Simpson_Area</t>
+  </si>
+  <si>
+    <t>Silicate_Trapezoid_Area</t>
+  </si>
+  <si>
+    <t>Silicate_Simpson_Area</t>
+  </si>
+  <si>
+    <t>Silicate_LHS_Back1</t>
+  </si>
+  <si>
+    <t>Silicate_LHS_Back2</t>
+  </si>
+  <si>
+    <t>Silicate_RHS_Back1</t>
+  </si>
+  <si>
+    <t>Silicate_RHS_Back2</t>
+  </si>
+  <si>
+    <t>Silicate_N_Poly</t>
+  </si>
+  <si>
+    <t>LW_Silicate_Trapezoid_Area</t>
+  </si>
+  <si>
+    <t>LW_Silicate_Simpson_Area</t>
+  </si>
+  <si>
+    <t>HW_Silicate_Trapezoid_Area</t>
+  </si>
+  <si>
+    <t>HW_Silicate_Simpson_Area</t>
+  </si>
+  <si>
+    <t>MW_Silicate_Trapezoid_Area</t>
+  </si>
+  <si>
+    <t>MW_Silicate_Simpson_Area</t>
+  </si>
+  <si>
+    <t>Water Filename</t>
+  </si>
+  <si>
+    <t>Water_LHS_Back1</t>
+  </si>
+  <si>
+    <t>Water_LHS_Back2</t>
+  </si>
+  <si>
+    <t>Water_RHS_Back1</t>
+  </si>
+  <si>
+    <t>Water_RHS_Back2</t>
+  </si>
+  <si>
+    <t>Water_N_Poly</t>
+  </si>
+  <si>
     <t>HW:LW_Trapezoid</t>
   </si>
   <si>
     <t>HW:LW_Simpson</t>
-  </si>
-  <si>
-    <t>Water_Trapezoid_Area</t>
-  </si>
-  <si>
-    <t>Water_Simpson_Area</t>
-  </si>
-  <si>
-    <t>Silicate_Trapezoid_Area</t>
-  </si>
-  <si>
-    <t>Silicate_Simpson_Area</t>
-  </si>
-  <si>
-    <t>Silicate_LHS_Back1</t>
-  </si>
-  <si>
-    <t>Silicate_LHS_Back2</t>
-  </si>
-  <si>
-    <t>Silicate_RHS_Back1</t>
-  </si>
-  <si>
-    <t>Silicate_RHS_Back2</t>
-  </si>
-  <si>
-    <t>Silicate_N_Poly</t>
-  </si>
-  <si>
-    <t>LW_Silicate_Trapezoid_Area</t>
-  </si>
-  <si>
-    <t>LW_Silicate_Simpson_Area</t>
-  </si>
-  <si>
-    <t>HW_Silicate_Trapezoid_Area</t>
-  </si>
-  <si>
-    <t>HW_Silicate_Simpson_Area</t>
-  </si>
-  <si>
-    <t>MW_Silicate_Trapezoid_Area</t>
-  </si>
-  <si>
-    <t>MW_Silicate_Simpson_Area</t>
-  </si>
-  <si>
-    <t>Water Filename</t>
-  </si>
-  <si>
-    <t>Water_LHS_Back1</t>
-  </si>
-  <si>
-    <t>Water_LHS_Back2</t>
-  </si>
-  <si>
-    <t>Water_RHS_Back1</t>
-  </si>
-  <si>
-    <t>Water_RHS_Back2</t>
-  </si>
-  <si>
-    <t>Water_N_Poly</t>
   </si>
   <si>
     <t>ETFS_OL39_MI7_50X_GLASS.txt</t>
@@ -452,13 +464,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:30">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,8 +546,20 @@
       <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:30">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -543,46 +567,46 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D2">
-        <v>3.928981975446791</v>
+        <v>1.035972117635653</v>
       </c>
       <c r="E2">
-        <v>3.928358555082121</v>
+        <v>1.036197547193371</v>
       </c>
       <c r="F2">
+        <v>0.7579678818556516</v>
+      </c>
+      <c r="G2">
+        <v>0.7576781215089602</v>
+      </c>
+      <c r="H2">
         <v>274807.3951902158</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>274611.0037276433</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>362558.1001103033</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>362437.5522164207</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>300</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>340</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>1200</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>1250</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>4</v>
-      </c>
-      <c r="O2">
-        <v>69943.66400954682</v>
-      </c>
-      <c r="P2">
-        <v>69904.77062547633</v>
       </c>
       <c r="Q2">
         <v>69943.66400954682</v>
@@ -591,31 +615,37 @@
         <v>69904.77062547633</v>
       </c>
       <c r="S2">
+        <v>265265.2426760239</v>
+      </c>
+      <c r="T2">
+        <v>265018.0020899012</v>
+      </c>
+      <c r="U2">
         <v>11333.3329334461</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>11224.56189991856</v>
       </c>
-      <c r="U2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2">
+      <c r="W2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2">
         <v>2500</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>2750</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>3750</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>4100</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:30">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -623,46 +653,34 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3">
-        <v>3.928981975446791</v>
-      </c>
-      <c r="E3">
-        <v>3.928358555082121</v>
-      </c>
-      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="H3">
         <v>274807.3951902158</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>274611.0037276433</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>362558.1001103033</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>362437.5522164207</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>300</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>340</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>1200</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>1250</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>4</v>
-      </c>
-      <c r="O3">
-        <v>69943.66400954682</v>
-      </c>
-      <c r="P3">
-        <v>69904.77062547633</v>
       </c>
       <c r="Q3">
         <v>69943.66400954682</v>
@@ -671,28 +689,40 @@
         <v>69904.77062547633</v>
       </c>
       <c r="S3">
+        <v>69943.66400954682</v>
+      </c>
+      <c r="T3">
+        <v>69904.77062547633</v>
+      </c>
+      <c r="U3">
         <v>11333.3329334461</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>11224.56189991856</v>
       </c>
-      <c r="U3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3">
+      <c r="W3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3">
         <v>2500</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>2750</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>3750</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>4100</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>3</v>
+      </c>
+      <c r="AC3">
+        <v>3.928981975446791</v>
+      </c>
+      <c r="AD3">
+        <v>3.928358555082121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>